<commit_message>
changed icon names and updated spreadsheet
</commit_message>
<xml_diff>
--- a/assets/spreadsheets/companyData.xlsx
+++ b/assets/spreadsheets/companyData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rinya\Projects\ABSA 2022\FrontEnd\FrontEnd\assets\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rinya\Projects\ABSA 2022\FrontEnd\absa_ecg_dashboard\assets\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E9058DE-C167-4DFB-85BE-E649DB7B41C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0A8B45-6B2D-40E8-802E-436DD86376C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2868" yWindow="1800" windowWidth="17280" windowHeight="8964" xr2:uid="{32B7449F-266E-46BC-B466-C6F9F7A78B7C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>SOUTH AFRICAN RUGBY UNION</t>
   </si>
@@ -149,6 +149,48 @@
   </si>
   <si>
     <t>1,986,711</t>
+  </si>
+  <si>
+    <t>Icon Src</t>
+  </si>
+  <si>
+    <t>/assets/icons/SARU_logo.svg</t>
+  </si>
+  <si>
+    <t>/assets/icons/afmetco-logo.png</t>
+  </si>
+  <si>
+    <t>/assets/icons/sagoodnews-pernod-ricard.png</t>
+  </si>
+  <si>
+    <t>/assets/icons/Nestle-Logo.png</t>
+  </si>
+  <si>
+    <t>/assets/icons/Country-Bird-Holdings.png</t>
+  </si>
+  <si>
+    <t>/assets/icons/karan_beef.png</t>
+  </si>
+  <si>
+    <t>/assets/icons/afgri-logo-for-posts.jpg</t>
+  </si>
+  <si>
+    <t>/assets/icons/homechoice.co.za.png</t>
+  </si>
+  <si>
+    <t>/assets/icons/telkom-logo.jpg</t>
+  </si>
+  <si>
+    <t>/assets/icons/vodacom.jpeg</t>
+  </si>
+  <si>
+    <t>/assets/icons/woolworths.jpeg</t>
+  </si>
+  <si>
+    <t>/assets/icons/mrprice.jpeg</t>
+  </si>
+  <si>
+    <t>/assets/icons/shoprite_checkers_logo.jpeg</t>
   </si>
 </sst>
 </file>
@@ -509,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB79C858-BD4B-4631-A1AB-B0E756FC2201}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,7 +566,7 @@
     <col min="5" max="5" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -549,8 +591,11 @@
       <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -575,8 +620,11 @@
       <c r="H2">
         <v>813</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -602,7 +650,7 @@
         <v>90700</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -628,7 +676,7 @@
         <v>318164</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -654,7 +702,7 @@
         <v>5652</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -679,8 +727,11 @@
       <c r="H6">
         <v>90850</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -705,8 +756,11 @@
       <c r="H7">
         <v>28924</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -731,8 +785,11 @@
       <c r="H8">
         <v>50882</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -758,7 +815,7 @@
         <v>23984</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -784,7 +841,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -809,8 +866,11 @@
       <c r="H11">
         <v>51400</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -835,8 +895,11 @@
       <c r="H12">
         <v>31838.609</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -861,8 +924,11 @@
       <c r="H13">
         <v>22963</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -887,8 +953,11 @@
       <c r="H14">
         <v>3275</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -913,8 +982,11 @@
       <c r="H15">
         <v>43034</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -939,8 +1011,11 @@
       <c r="H16">
         <v>90746</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -965,8 +1040,11 @@
       <c r="H17">
         <v>919.75099999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -991,8 +1069,11 @@
       <c r="H18">
         <v>22963</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1017,8 +1098,12 @@
       <c r="H19">
         <v>155409</v>
       </c>
+      <c r="I19" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
charts and series added to lib/bar_charts
</commit_message>
<xml_diff>
--- a/assets/spreadsheets/companyData.xlsx
+++ b/assets/spreadsheets/companyData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rinya\Projects\ABSA 2022\FrontEnd\absa_ecg_dashboard\assets\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joelle Behoor\Desktop\StatisticalComputing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0A8B45-6B2D-40E8-802E-436DD86376C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="269" documentId="13_ncr:1_{3469AE54-0B51-4AFA-8324-044C4A5FB360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7AA05C6-A48C-46EB-B19C-C74506AB3FD4}"/>
   <bookViews>
-    <workbookView xWindow="2868" yWindow="1800" windowWidth="17280" windowHeight="8964" xr2:uid="{32B7449F-266E-46BC-B466-C6F9F7A78B7C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{32B7449F-266E-46BC-B466-C6F9F7A78B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,16 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
-  <si>
-    <t>SOUTH AFRICAN RUGBY UNION</t>
-  </si>
-  <si>
-    <t>PROFESSIONAL SERVICES</t>
-  </si>
-  <si>
-    <t>CORPORATE LIQUIDATORS (PTY) LTD</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Client Name</t>
   </si>
@@ -70,16 +61,25 @@
     <t xml:space="preserve"> 2020 Revenue (Rm)</t>
   </si>
   <si>
-    <t>CHEMWES (PTY) LTD</t>
+    <t>FNB</t>
+  </si>
+  <si>
+    <t>Banking</t>
+  </si>
+  <si>
+    <t>Nedbank</t>
+  </si>
+  <si>
+    <t>ANGLO AMERICAN (PTY) LTD</t>
   </si>
   <si>
     <t>MINING &amp; METALS</t>
   </si>
   <si>
-    <t>RICHARDS BAY TITANIUM (PTY) LTD</t>
-  </si>
-  <si>
-    <t>AFMETCO (PTY) LTD</t>
+    <t>NAWA</t>
+  </si>
+  <si>
+    <t>Exarro SA</t>
   </si>
   <si>
     <t>PERNOD RICARD SOUTH AFRICA (PTY) LTD</t>
@@ -91,113 +91,71 @@
     <t>NESTLE (SOUTH AFRICA) (PTY) LTD</t>
   </si>
   <si>
-    <t>WORLD HARDWOOD (PTY) LTD</t>
+    <t>MBALI</t>
   </si>
   <si>
     <t>ISUZU MOTORS(SOUTH AFRICA)(PTY)(LTD)</t>
   </si>
   <si>
-    <t xml:space="preserve">13 68 </t>
-  </si>
-  <si>
-    <t>12 67</t>
-  </si>
-  <si>
     <t>COUNTRY BIRD HOLDINGS (PTY) LTD</t>
   </si>
   <si>
     <t>AGRICULTURE</t>
   </si>
   <si>
+    <t>NSUKU</t>
+  </si>
+  <si>
     <t>KARAN BEEF FEEDLOT</t>
   </si>
   <si>
     <t>AFGRI GRAIN MARKETING (PTY) LTD</t>
   </si>
   <si>
-    <t>HOMECHOICE (PTY)LTD</t>
+    <t>NDZALO</t>
+  </si>
+  <si>
+    <t>MTN</t>
   </si>
   <si>
     <t>TMT</t>
   </si>
   <si>
-    <t>671.1640</t>
-  </si>
-  <si>
-    <t>18933.50141</t>
-  </si>
-  <si>
     <t>TELKOM SA SOC LTD</t>
   </si>
   <si>
+    <t>JO</t>
+  </si>
+  <si>
     <t>VODACOM(PTY) LTD</t>
   </si>
   <si>
-    <t xml:space="preserve">Woolworths group </t>
+    <t>WOOLWORTHS HOLDINGS LIMITED</t>
   </si>
   <si>
     <t>RETAIL</t>
   </si>
   <si>
+    <t>AMANDA</t>
+  </si>
+  <si>
     <t>MR PRICE GROUP LTD</t>
   </si>
   <si>
-    <t>SHOPRITE CHECKERS (PTY)LTD</t>
-  </si>
-  <si>
-    <t>1,867,528</t>
-  </si>
-  <si>
-    <t>1,986,711</t>
-  </si>
-  <si>
-    <t>Icon Src</t>
-  </si>
-  <si>
-    <t>/assets/icons/SARU_logo.svg</t>
-  </si>
-  <si>
-    <t>/assets/icons/afmetco-logo.png</t>
-  </si>
-  <si>
-    <t>/assets/icons/sagoodnews-pernod-ricard.png</t>
-  </si>
-  <si>
-    <t>/assets/icons/Nestle-Logo.png</t>
-  </si>
-  <si>
-    <t>/assets/icons/Country-Bird-Holdings.png</t>
-  </si>
-  <si>
-    <t>/assets/icons/karan_beef.png</t>
-  </si>
-  <si>
-    <t>/assets/icons/afgri-logo-for-posts.jpg</t>
-  </si>
-  <si>
-    <t>/assets/icons/homechoice.co.za.png</t>
-  </si>
-  <si>
-    <t>/assets/icons/telkom-logo.jpg</t>
-  </si>
-  <si>
-    <t>/assets/icons/vodacom.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/icons/woolworths.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/icons/mrprice.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/icons/shoprite_checkers_logo.jpeg</t>
+    <t>SHOPRITE HOLDINGS</t>
+  </si>
+  <si>
+    <t>MATTHEW</t>
+  </si>
+  <si>
+    <t>IMPLATS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,9 +192,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,559 +515,778 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB79C858-BD4B-4631-A1AB-B0E756FC2201}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="C2">
+        <v>6507</v>
+      </c>
+      <c r="D2" s="2">
+        <v>153</v>
+      </c>
+      <c r="E2">
+        <v>24</v>
+      </c>
+      <c r="F2">
+        <v>8301</v>
+      </c>
+      <c r="G2" s="2">
+        <v>171</v>
+      </c>
+      <c r="H2" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>283.60630722278739</v>
-      </c>
-      <c r="D2">
-        <v>3101.4191251271618</v>
-      </c>
-      <c r="E2">
-        <v>500</v>
-      </c>
-      <c r="F2">
-        <v>484.66273428886444</v>
-      </c>
-      <c r="G2">
-        <v>4991.1387651598679</v>
-      </c>
-      <c r="H2">
-        <v>813</v>
-      </c>
-      <c r="I2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="B3" t="str">
+        <f>B2</f>
+        <v>Banking</v>
       </c>
       <c r="C3">
-        <v>55757</v>
+        <v>1541</v>
       </c>
       <c r="D3">
-        <v>609739</v>
-      </c>
-      <c r="E3">
-        <v>98300</v>
+        <v>110529</v>
+      </c>
+      <c r="E3" s="2">
+        <v>25</v>
       </c>
       <c r="F3">
-        <v>54070</v>
+        <v>1265</v>
       </c>
       <c r="G3">
-        <v>556822</v>
-      </c>
-      <c r="H3">
-        <v>90700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>118050</v>
+      </c>
+      <c r="H3" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
-        <v>72055.000438849747</v>
-      </c>
-      <c r="D4">
-        <v>492873.43120452709</v>
-      </c>
-      <c r="E4">
-        <v>282536</v>
-      </c>
-      <c r="F4">
-        <v>72808.250522839851</v>
-      </c>
-      <c r="G4">
-        <v>551122.38503026974</v>
-      </c>
-      <c r="H4">
-        <v>318164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C4" s="3">
+        <v>875714.28571428568</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1428571.4285714286</v>
+      </c>
+      <c r="E4" s="3">
+        <v>4414.2857142857147</v>
+      </c>
+      <c r="F4" s="3">
+        <v>875714.28571428568</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1428571.4285714286</v>
+      </c>
+      <c r="H4" s="3">
+        <v>96285.71428571429</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5">
-        <v>1263.1608615313546</v>
+        <v>345000</v>
       </c>
       <c r="D5">
-        <v>8640.3223120452712</v>
+        <v>650000</v>
       </c>
       <c r="E5">
-        <v>4953</v>
+        <v>32771</v>
       </c>
       <c r="F5">
-        <v>1293.3965877820583</v>
+        <v>385000</v>
       </c>
       <c r="G5">
-        <v>9790.3713813979084</v>
+        <v>650000</v>
       </c>
       <c r="H5">
-        <v>5652</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>28924</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>22083</v>
+        <v>345</v>
       </c>
       <c r="D6">
-        <v>151053</v>
+        <v>650</v>
       </c>
       <c r="E6">
-        <v>86590</v>
+        <v>3424</v>
       </c>
       <c r="F6">
-        <v>20790</v>
+        <v>385</v>
       </c>
       <c r="G6">
-        <v>157370</v>
+        <v>1035</v>
       </c>
       <c r="H6">
-        <v>90850</v>
-      </c>
-      <c r="I6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4818</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7">
-        <v>345</v>
+        <v>730</v>
       </c>
       <c r="D7">
-        <v>650</v>
+        <v>1375</v>
       </c>
       <c r="E7">
-        <v>32771</v>
+        <v>7241</v>
       </c>
       <c r="F7">
-        <v>385</v>
+        <v>579</v>
       </c>
       <c r="G7">
-        <v>1035</v>
+        <v>1555</v>
       </c>
       <c r="H7">
-        <v>28924</v>
-      </c>
-      <c r="I7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7240</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="C8">
-        <v>1127.2744194562265</v>
+        <v>78709</v>
       </c>
       <c r="D8">
-        <v>2123.8503554972385</v>
+        <v>353716</v>
       </c>
       <c r="E8">
-        <v>107078</v>
+        <v>2257</v>
       </c>
       <c r="F8">
-        <v>677.27734753146183</v>
+        <v>71598</v>
       </c>
       <c r="G8">
-        <v>1820.7326095975661</v>
+        <v>371340</v>
       </c>
       <c r="H8">
-        <v>50882</v>
-      </c>
-      <c r="I8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2515</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C9">
-        <v>0.27664428915809708</v>
+        <v>15837</v>
       </c>
       <c r="D9">
-        <v>0.52121387812395104</v>
+        <v>52010</v>
       </c>
       <c r="E9">
-        <v>26.277999999999999</v>
+        <v>2359</v>
       </c>
       <c r="F9">
-        <v>319.24491771539203</v>
+        <v>19221</v>
       </c>
       <c r="G9">
-        <v>858.22984372839164</v>
+        <v>57500</v>
       </c>
       <c r="H9">
-        <v>23984</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2685</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>78709</v>
+        <v>228075</v>
       </c>
       <c r="D10">
-        <v>353716</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
+        <v>749018</v>
+      </c>
+      <c r="E10">
+        <v>33973</v>
       </c>
       <c r="F10">
-        <v>71598</v>
+        <v>12649</v>
       </c>
       <c r="G10">
-        <v>371340</v>
-      </c>
-      <c r="H10" t="s">
+        <v>37840</v>
+      </c>
+      <c r="H10">
+        <v>1767</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
       <c r="C11">
-        <v>15837</v>
+        <v>153247</v>
       </c>
       <c r="D11">
-        <v>52010</v>
+        <v>503277</v>
       </c>
       <c r="E11">
-        <v>53400</v>
+        <v>22827</v>
       </c>
       <c r="F11">
-        <v>19221</v>
+        <v>164384</v>
       </c>
       <c r="G11">
-        <v>57500</v>
+        <v>491758</v>
       </c>
       <c r="H11">
-        <v>51400</v>
-      </c>
-      <c r="I11" t="s">
+        <v>22963</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <v>566785</v>
+      </c>
+      <c r="D12">
+        <v>566785</v>
+      </c>
+      <c r="E12">
+        <v>181646</v>
+      </c>
+      <c r="F12">
+        <v>247385</v>
+      </c>
+      <c r="G12">
+        <v>864865</v>
+      </c>
+      <c r="H12">
+        <v>179361</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>50695</v>
+      </c>
+      <c r="D13">
+        <v>57825</v>
+      </c>
+      <c r="E13">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12">
-        <v>10075.631078426966</v>
-      </c>
-      <c r="D12">
-        <v>33089.194442696629</v>
-      </c>
-      <c r="E12">
-        <v>33973.523999999998</v>
-      </c>
-      <c r="F12">
-        <v>11906.02925270428</v>
-      </c>
-      <c r="G12">
-        <v>35617.12096303502</v>
-      </c>
-      <c r="H12">
-        <v>31838.609</v>
-      </c>
-      <c r="I12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13">
-        <v>6769.8726404494382</v>
-      </c>
-      <c r="D13">
-        <v>22232.814044943822</v>
-      </c>
-      <c r="E13">
-        <v>22827</v>
-      </c>
       <c r="F13">
-        <v>8587.0004474708167</v>
+        <v>50101</v>
       </c>
       <c r="G13">
-        <v>25688.180933852142</v>
+        <v>546000</v>
       </c>
       <c r="H13">
-        <v>22963</v>
-      </c>
-      <c r="I13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" t="s">
-        <v>29</v>
+      <c r="C14">
+        <v>55757</v>
+      </c>
+      <c r="D14">
+        <v>553982</v>
       </c>
       <c r="E14">
-        <v>3.4319999999999999</v>
+        <v>98</v>
       </c>
       <c r="F14">
-        <v>1.9510000000000001</v>
+        <v>54070</v>
       </c>
       <c r="G14">
-        <v>20.096</v>
+        <v>556822</v>
       </c>
       <c r="H14">
-        <v>3275</v>
-      </c>
-      <c r="I14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C15">
-        <v>50695</v>
+        <v>449819</v>
       </c>
       <c r="D15">
-        <v>57825</v>
-      </c>
-      <c r="E15">
-        <v>43.222000000000001</v>
+        <v>40675226</v>
+      </c>
+      <c r="E15" s="5">
+        <v>80942</v>
       </c>
       <c r="F15">
-        <v>55227</v>
+        <v>44886</v>
       </c>
       <c r="G15">
-        <v>601433</v>
+        <v>441875</v>
       </c>
       <c r="H15">
-        <v>43034</v>
-      </c>
-      <c r="I15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>74058</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C16">
-        <v>19224</v>
+        <v>46034</v>
       </c>
       <c r="D16">
-        <v>542308</v>
+        <v>46034</v>
       </c>
       <c r="E16">
-        <v>98.302000000000007</v>
+        <v>22306</v>
       </c>
       <c r="F16">
-        <v>54.07</v>
+        <v>52535</v>
       </c>
       <c r="G16">
-        <v>556.822</v>
+        <v>52535</v>
       </c>
       <c r="H16">
-        <v>90746</v>
-      </c>
-      <c r="I16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>22963</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
       <c r="C17">
-        <v>981235</v>
+        <v>511067</v>
       </c>
       <c r="D17">
-        <v>981235</v>
+        <v>1694193</v>
       </c>
       <c r="E17">
-        <v>790.84199999999998</v>
+        <v>171188</v>
       </c>
       <c r="F17">
-        <v>1022899.9999999999</v>
+        <v>528889</v>
       </c>
       <c r="G17">
-        <v>1022899.9999999999</v>
+        <v>1802314</v>
       </c>
       <c r="H17">
-        <v>919.75099999999998</v>
-      </c>
-      <c r="I17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>158310</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C18">
-        <v>50000</v>
+        <v>447247</v>
       </c>
       <c r="D18">
-        <v>50000</v>
+        <v>3307630</v>
       </c>
       <c r="E18">
-        <v>22306</v>
+        <v>129575</v>
       </c>
       <c r="F18">
-        <v>60000</v>
+        <v>380114</v>
       </c>
       <c r="G18">
-        <v>60000</v>
+        <v>2925700</v>
       </c>
       <c r="H18">
-        <v>22963</v>
-      </c>
-      <c r="I18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19">
-        <v>563355</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19">
-        <v>168030</v>
-      </c>
-      <c r="F19">
-        <v>583000</v>
-      </c>
-      <c r="G19" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19">
-        <v>155409</v>
-      </c>
-      <c r="I19" t="s">
-        <v>51</v>
-      </c>
+        <v>69851</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="I13:J14"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="I17:J18"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J8"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="I11:J12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="09e1d977-951d-4bc6-86f9-445f1353ea6b">
+      <UserInfo>
+        <DisplayName>Joelle Behoor</DisplayName>
+        <AccountId>18</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Amanda Maseko</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010083898A013DFF204486203E91027053DB" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fd7be6095bdaacbdb669932f905ad849">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dd2ed3c3-6d28-42e0-ab74-0b26c2c461e6" xmlns:ns3="09e1d977-951d-4bc6-86f9-445f1353ea6b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e0fcac0684ae2bad642bd46da616d01" ns2:_="" ns3:_="">
+    <xsd:import namespace="dd2ed3c3-6d28-42e0-ab74-0b26c2c461e6"/>
+    <xsd:import namespace="09e1d977-951d-4bc6-86f9-445f1353ea6b"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="dd2ed3c3-6d28-42e0-ab74-0b26c2c461e6" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="09e1d977-951d-4bc6-86f9-445f1353ea6b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADFA84AE-E621-4AC9-BBB4-646B05979E7A}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6ABB33F-D454-4E20-A57E-AF13BF0E5585}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{943F825D-C149-430E-8874-C6F4E61DDC91}"/>
 </file>
</xml_diff>